<commit_message>
a lot of progress done on the presentation
</commit_message>
<xml_diff>
--- a/reporte_estadistico/data/energia/metrics_data_fac.xlsx
+++ b/reporte_estadistico/data/energia/metrics_data_fac.xlsx
@@ -1,21 +1,94 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\JJ\repos\research_eslatina\reporte_estadistico\data\energia\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="236" yWindow="13" windowWidth="16089" windowHeight="9661"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>quant0</t>
+  </si>
+  <si>
+    <t>quant25</t>
+  </si>
+  <si>
+    <t>quant50</t>
+  </si>
+  <si>
+    <t>quant75</t>
+  </si>
+  <si>
+    <t>quant100</t>
+  </si>
+  <si>
+    <t>skewness</t>
+  </si>
+  <si>
+    <t>kurtosis</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>std_dev</t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Estrato1_fac</t>
+  </si>
+  <si>
+    <t>Estrato2_fac</t>
+  </si>
+  <si>
+    <t>Estrato3_fac</t>
+  </si>
+  <si>
+    <t>Estrato4_fac</t>
+  </si>
+  <si>
+    <t>Estrato5_fac</t>
+  </si>
+  <si>
+    <t>Estrato6_fac</t>
+  </si>
+  <si>
+    <t>totResidencial_fac</t>
+  </si>
+  <si>
+    <t>totNoResidencial_fac</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,11 +136,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +222,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +257,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,104 +433,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>quant0</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>quant25</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>quant50</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>quant75</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>quant100</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>skewness</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>kurtosis</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>median</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>std_dev</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>variance</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Estrato1_fac</t>
-        </is>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2">
         <v>-294.69619</v>
       </c>
       <c r="C2">
-        <v>231.8981265</v>
+        <v>231.89812649999999</v>
       </c>
       <c r="D2">
-        <v>861.620918</v>
+        <v>861.62091799999996</v>
       </c>
       <c r="E2">
-        <v>2930.64437496</v>
+        <v>2930.6443749599998</v>
       </c>
       <c r="F2">
-        <v>254971.44370214</v>
+        <v>254971.44370214001</v>
       </c>
       <c r="G2">
-        <v>1.436265265146852</v>
+        <v>1.4362652651468519</v>
       </c>
       <c r="H2">
-        <v>4.142432570409112</v>
+        <v>4.1424325704091123</v>
       </c>
       <c r="I2">
-        <v>861.620918</v>
+        <v>861.62091799999996</v>
       </c>
       <c r="J2">
         <v>15646.26908457299</v>
@@ -456,63 +518,67 @@
         <v>244805736.2668646</v>
       </c>
       <c r="L2">
-        <v>4271.098748815498</v>
+        <v>4271.0987488154979</v>
+      </c>
+      <c r="M2">
+        <f>J2/L2</f>
+        <v>3.663289004711531</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Estrato2_fac</t>
-        </is>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>420.341698</v>
+        <v>420.34169800000001</v>
       </c>
       <c r="D3">
-        <v>974.135466</v>
+        <v>974.13546599999995</v>
       </c>
       <c r="E3">
         <v>2649.670267</v>
       </c>
       <c r="F3">
-        <v>750281.955535</v>
+        <v>750281.95553499996</v>
       </c>
       <c r="G3">
         <v>1.494178783098568</v>
       </c>
       <c r="H3">
-        <v>4.604189217332683</v>
+        <v>4.6041892173326833</v>
       </c>
       <c r="I3">
-        <v>974.135466</v>
+        <v>974.13546599999995</v>
       </c>
       <c r="J3">
-        <v>26618.32216609362</v>
+        <v>26618.322166093621</v>
       </c>
       <c r="K3">
-        <v>708535074.9379509</v>
+        <v>708535074.93795085</v>
       </c>
       <c r="L3">
         <v>4640.944790129628</v>
       </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M9" si="0">J3/L3</f>
+        <v>5.7355395010743351</v>
+      </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Estrato3_fac</t>
-        </is>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>7.977563865000001</v>
+        <v>7.9775638650000014</v>
       </c>
       <c r="D4">
-        <v>64.519251</v>
+        <v>64.519250999999997</v>
       </c>
       <c r="E4">
         <v>560.7229225000001</v>
@@ -521,32 +587,34 @@
         <v>754861.455953</v>
       </c>
       <c r="G4">
-        <v>2.255631030411629</v>
+        <v>2.2556310304116289</v>
       </c>
       <c r="H4">
-        <v>7.703684712414301</v>
+        <v>7.7036847124143009</v>
       </c>
       <c r="I4">
-        <v>64.519251</v>
+        <v>64.519250999999997</v>
       </c>
       <c r="J4">
         <v>26931.35412904403</v>
       </c>
       <c r="K4">
-        <v>725297835.2239767</v>
+        <v>725297835.22397673</v>
       </c>
       <c r="L4">
         <v>3005.404405556847</v>
       </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>8.9609751284217403</v>
+      </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Estrato4_fac</t>
-        </is>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>-0.154485</v>
+        <v>-0.15448500000000001</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -555,22 +623,22 @@
         <v>2.218064</v>
       </c>
       <c r="E5">
-        <v>43.597984025</v>
+        <v>43.597984025000002</v>
       </c>
       <c r="F5">
-        <v>305949.310939</v>
+        <v>305949.31093899999</v>
       </c>
       <c r="G5">
         <v>3.329749869162336</v>
       </c>
       <c r="H5">
-        <v>14.37734785014072</v>
+        <v>14.377347850140721</v>
       </c>
       <c r="I5">
         <v>2.218064</v>
       </c>
       <c r="J5">
-        <v>11161.4909181428</v>
+        <v>11161.490918142799</v>
       </c>
       <c r="K5">
         <v>124578879.5157842</v>
@@ -578,15 +646,17 @@
       <c r="L5">
         <v>1168.738688453795</v>
       </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>9.5500311818282544</v>
+      </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Estrato5_fac</t>
-        </is>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>-1.557759</v>
+        <v>-1.5577589999999999</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -595,13 +665,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>3.2083535</v>
+        <v>3.2083534999999999</v>
       </c>
       <c r="F6">
-        <v>126291.349364</v>
+        <v>126291.34936399999</v>
       </c>
       <c r="G6">
-        <v>4.000254710268297</v>
+        <v>4.0002547102682966</v>
       </c>
       <c r="H6">
         <v>20.58755726482919</v>
@@ -610,20 +680,22 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>5524.792573279144</v>
+        <v>5524.7925732791437</v>
       </c>
       <c r="K6">
-        <v>30523332.97776038</v>
+        <v>30523332.977760378</v>
       </c>
       <c r="L6">
-        <v>529.8101275832</v>
+        <v>529.81012758320003</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>10.427872714478347</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Estrato6_fac</t>
-        </is>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -638,105 +710,113 @@
         <v>1.1519085</v>
       </c>
       <c r="F7">
-        <v>137518.126014</v>
+        <v>137518.12601400001</v>
       </c>
       <c r="G7">
-        <v>4.121199893104263</v>
+        <v>4.1211998931042633</v>
       </c>
       <c r="H7">
-        <v>20.77211138929474</v>
+        <v>20.772111389294739</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>5483.600377120617</v>
+        <v>5483.6003771206169</v>
       </c>
       <c r="K7">
-        <v>30069873.09595737</v>
+        <v>30069873.095957369</v>
       </c>
       <c r="L7">
-        <v>465.3570871937674</v>
+        <v>465.35708719376743</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>11.783639978899325</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>totResidencial_fac</t>
-        </is>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>67.568932</v>
+        <v>67.568932000000004</v>
       </c>
       <c r="C8">
-        <v>731.101801</v>
+        <v>731.10180100000002</v>
       </c>
       <c r="D8">
         <v>1757.398408</v>
       </c>
       <c r="E8">
-        <v>5050.0859385</v>
+        <v>5050.0859385000003</v>
       </c>
       <c r="F8">
         <v>1884225.012473</v>
       </c>
       <c r="G8">
-        <v>1.823155916861877</v>
+        <v>1.8231559168618769</v>
       </c>
       <c r="H8">
-        <v>6.001998066912449</v>
+        <v>6.0019980669124493</v>
       </c>
       <c r="I8">
         <v>1757.398408</v>
       </c>
       <c r="J8">
-        <v>73296.82750134372</v>
+        <v>73296.827501343723</v>
       </c>
       <c r="K8">
-        <v>5372424921.761738</v>
+        <v>5372424921.7617378</v>
       </c>
       <c r="L8">
-        <v>12125.86043944744</v>
+        <v>12125.860439447441</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>6.04467022091867</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>totNoResidencial_fac</t>
-        </is>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
       </c>
       <c r="B9">
         <v>11.707744</v>
       </c>
       <c r="C9">
-        <v>526.7598135000001</v>
+        <v>526.75981350000006</v>
       </c>
       <c r="D9">
-        <v>1450.255466</v>
+        <v>1450.2554660000001</v>
       </c>
       <c r="E9">
-        <v>4483.8118775</v>
+        <v>4483.8118775000003</v>
       </c>
       <c r="F9">
-        <v>9093718.742579</v>
+        <v>9093718.7425790001</v>
       </c>
       <c r="G9">
         <v>2.137569141671726</v>
       </c>
       <c r="H9">
-        <v>7.499561962213636</v>
+        <v>7.4995619622136358</v>
       </c>
       <c r="I9">
-        <v>1450.255466</v>
+        <v>1450.2554660000001</v>
       </c>
       <c r="J9">
-        <v>286390.3117818618</v>
+        <v>286390.31178186182</v>
       </c>
       <c r="K9">
-        <v>82019410682.51198</v>
+        <v>82019410682.511978</v>
       </c>
       <c r="L9">
-        <v>19901.75249271512</v>
+        <v>19901.752492715121</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>14.390205680966675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>